<commit_message>
pdf results generation, new add to database script, and frontend work
</commit_message>
<xml_diff>
--- a/sample-questions.xlsx
+++ b/sample-questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benis\Desktop\Git Projects\online-testing-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52B245F1-E799-48CC-BED0-C03C2F38B8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4962AAF7-E0F7-4C5C-9FD9-7EDF50B243D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{76A6AFED-8A09-4196-9104-73E30702A971}"/>
+    <workbookView minimized="1" xWindow="4545" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{76A6AFED-8A09-4196-9104-73E30702A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
   <si>
     <t>Section</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t xml:space="preserve">D </t>
+  </si>
+  <si>
+    <t>Exam Name</t>
+  </si>
+  <si>
+    <t>mock exam1</t>
   </si>
 </sst>
 </file>
@@ -667,456 +673,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABD6CE4-6DBD-4324-95C0-5CDF64E11C4A}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="78.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>47</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>52</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>54</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
         <v>9</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>63</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>68</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>72</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>73</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>76</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>77</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>78</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>15</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>20</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>84</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>6</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>16</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added primitive version of reading passages and changed question model to have a 'material' field
</commit_message>
<xml_diff>
--- a/sample-questions.xlsx
+++ b/sample-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benis\Desktop\Git Projects\online-testing-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ADD89D-2C96-46F6-8C46-D42C8217A94D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3373B0-FAE0-4DD5-B179-168E2797DE30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{76A6AFED-8A09-4196-9104-73E30702A971}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Section</t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>no question3</t>
+  </si>
+  <si>
+    <t>has_material</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -682,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABD6CE4-6DBD-4324-95C0-5CDF64E11C4A}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,13 +702,13 @@
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -721,8 +730,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -744,8 +756,11 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -764,8 +779,11 @@
       <c r="G3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -784,8 +802,11 @@
       <c r="G4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -804,8 +825,11 @@
       <c r="G5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -824,8 +848,11 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -844,8 +871,11 @@
       <c r="G7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -864,8 +894,11 @@
       <c r="G8" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -884,8 +917,11 @@
       <c r="G9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -904,8 +940,11 @@
       <c r="G10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -924,8 +963,11 @@
       <c r="G11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -944,8 +986,11 @@
       <c r="G12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -964,8 +1009,11 @@
       <c r="G13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -984,8 +1032,11 @@
       <c r="G14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -1004,8 +1055,11 @@
       <c r="G15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -1024,8 +1078,11 @@
       <c r="G16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>9</v>
       </c>
@@ -1044,8 +1101,11 @@
       <c r="G17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -1064,8 +1124,11 @@
       <c r="G18" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -1084,8 +1147,11 @@
       <c r="G19" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1104,8 +1170,11 @@
       <c r="G20" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -1124,22 +1193,25 @@
       <c r="G21" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>

</xml_diff>

<commit_message>
Added MathJax functionality and improved file uploading infrastructure
</commit_message>
<xml_diff>
--- a/sample-questions.xlsx
+++ b/sample-questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benis\Desktop\Git Projects\online-testing-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3373B0-FAE0-4DD5-B179-168E2797DE30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2925C9-0873-4E9D-A0AA-B6EFCC96FB64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{76A6AFED-8A09-4196-9104-73E30702A971}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{76A6AFED-8A09-4196-9104-73E30702A971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
   <si>
     <t>Section</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>math2</t>
-  </si>
-  <si>
-    <t>Which choice best describes what happens in the passage?</t>
   </si>
   <si>
     <t>One character argues with another character who intrudes on her home</t>
@@ -330,13 +327,11 @@
     <t>no question3</t>
   </si>
   <si>
-    <t>has_material</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>Passage</t>
+  </si>
+  <si>
+    <t>When \(a \ne 0\), there are two solutions to \(ax^2 + bx + c = 0\) and they are
+$$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
   </si>
 </sst>
 </file>
@@ -693,530 +688,500 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABD6CE4-6DBD-4324-95C0-5CDF64E11C4A}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>37</v>
       </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>44</v>
-      </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
         <v>46</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>51</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>52</v>
-      </c>
-      <c r="G11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
+      <c r="D12" t="s">
+        <v>53</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
         <v>9</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>58</v>
-      </c>
-      <c r="G13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>62</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>63</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>68</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>71</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>72</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>73</v>
-      </c>
-      <c r="G16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
         <v>75</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>76</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>78</v>
-      </c>
-      <c r="G17" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1">
         <v>6</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>15</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>20</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>23</v>
-      </c>
-      <c r="H18" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
         <v>81</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>82</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>83</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>84</v>
-      </c>
-      <c r="G19" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>6</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>16</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>80</v>
       </c>
-      <c r="H20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>